<commit_message>
fixing gcrmn ecoregion assignments for ropme
</commit_message>
<xml_diff>
--- a/data_raw/spatial/ecoregions/gcrmn_meow_ecoregions.xlsx
+++ b/data_raw/spatial/ecoregions/gcrmn_meow_ecoregions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzinho/Desktop/research/cordio-ea_iucn_red-list-ecosystems_public/data_raw/spatial/ecoregions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzinho/Desktop/research/cordio-ea_iucn_regional-rle_coral_reefs_ropme/data_raw/spatial/ecoregions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE97AECF-6FC8-B841-83F9-E1CE001863FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909C0D30-A625-1949-A1A6-80E0D33C2CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20540" yWindow="800" windowWidth="21880" windowHeight="24160" xr2:uid="{9927B8F5-5E57-AB43-8D87-6E0E4C0C63E5}"/>
   </bookViews>
@@ -932,8 +932,8 @@
   <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1639,10 +1639,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>103</v>
@@ -1650,10 +1650,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>105</v>
@@ -1661,10 +1661,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>107</v>
@@ -1672,10 +1672,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>110</v>
@@ -1683,10 +1683,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>112</v>
@@ -1694,10 +1694,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
reviewing creation code for criterion d fish consumers
</commit_message>
<xml_diff>
--- a/data_raw/spatial/ecoregions/gcrmn_meow_ecoregions.xlsx
+++ b/data_raw/spatial/ecoregions/gcrmn_meow_ecoregions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzinho/Desktop/research/cordio-ea_iucn_regional-rle_coral_reefs_ropme/data_raw/spatial/ecoregions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909C0D30-A625-1949-A1A6-80E0D33C2CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83809A0C-4132-A442-94F0-4A4D40EA7C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20540" yWindow="800" windowWidth="21880" windowHeight="24160" xr2:uid="{9927B8F5-5E57-AB43-8D87-6E0E4C0C63E5}"/>
   </bookViews>
@@ -932,8 +932,8 @@
   <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67:XFD69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1639,10 +1639,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>103</v>
@@ -1650,10 +1650,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>105</v>
@@ -1661,10 +1661,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>107</v>
@@ -1672,10 +1672,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>110</v>
@@ -1683,10 +1683,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>112</v>
@@ -1694,10 +1694,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>114</v>

</xml_diff>